<commit_message>
add the bood add system
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_NardouThomas.xlsx
+++ b/Doc/Journal-de-Travail_NardouThomas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pk88yte\Documents\GitHub\Passion-Book-Mobile\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CFAAE3-8FB0-42F8-BFD2-F64B3BB8F3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5092D4-6BAF-4B76-81F4-9780E50CCB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -154,6 +154,30 @@
   </si>
   <si>
     <t xml:space="preserve">J'ai continuer de paufiner quelque petit détails pour la page d'accueil </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai fait des recherches pour un border radius et le click event sur un autre élément qu'un bouton </t>
+  </si>
+  <si>
+    <t>J'ai continuer a faire de rechercher et tester ce que j'ai appris pour passer des paramètre lors du changement de page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je continue d'avancer sur le problème en essayer d'ajouter un nouveau livre sur l'application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai commencé à modifier mon API pour qu'elle puisse recevoir des fichier </t>
+  </si>
+  <si>
+    <t>j'AI CONTUNIER A DOCKERISé L'API MAIS SANS SUCCèS DUCOUP JE SUIS RETOURNER AVANCé SUR L'APPLICATION MOBILE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">au final je continue mes recheres sur la connexions avec l'API </t>
+  </si>
+  <si>
+    <t>J'ai essayé de connecter mon application avec l'API (avec M. Melly)</t>
+  </si>
+  <si>
+    <t>Avec M. melly nous avons continuer d'essayer de connecter l'application avec l'API mais sans succès</t>
   </si>
 </sst>
 </file>
@@ -1048,7 +1072,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24652777777777779</c:v>
+                  <c:v>0.37152777777777779</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1978,8 +2002,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2032,7 +2056,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 9 heurs 55 minutes</v>
+        <v>0 jours 12 heurs 55 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2051,11 +2075,11 @@
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>175</v>
+        <v>355</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>595</v>
+        <v>775</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2294,7 +2318,9 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
-      <c r="B15" s="40"/>
+      <c r="B15" s="40">
+        <v>45397</v>
+      </c>
       <c r="C15" s="36"/>
       <c r="D15" s="44">
         <v>20</v>
@@ -2317,32 +2343,58 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="39"/>
+      <c r="B16" s="39">
+        <v>45404</v>
+      </c>
       <c r="C16" s="35"/>
-      <c r="D16" s="43"/>
-      <c r="F16" s="48"/>
+      <c r="D16" s="43">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="17"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
-      <c r="B17" s="40"/>
+      <c r="B17" s="40">
+        <v>45404</v>
+      </c>
       <c r="C17" s="36"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="48"/>
+      <c r="D17" s="44">
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>39</v>
+      </c>
       <c r="G17" s="20"/>
       <c r="O17">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="39"/>
+      <c r="B18" s="39">
+        <v>45404</v>
+      </c>
       <c r="C18" s="35"/>
-      <c r="D18" s="43"/>
-      <c r="F18" s="48"/>
+      <c r="D18" s="43">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="48" t="s">
+        <v>40</v>
+      </c>
       <c r="G18" s="17"/>
       <c r="O18">
         <v>50</v>
@@ -2350,46 +2402,88 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
-      <c r="B19" s="40"/>
+      <c r="B19" s="40">
+        <v>45404</v>
+      </c>
       <c r="C19" s="36"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="48"/>
+      <c r="D19" s="44">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="48" t="s">
+        <v>41</v>
+      </c>
       <c r="G19" s="20"/>
       <c r="O19">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="39"/>
+    <row r="20" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B20" s="39">
+        <v>45404</v>
+      </c>
       <c r="C20" s="35"/>
-      <c r="D20" s="43"/>
-      <c r="F20" s="48"/>
+      <c r="D20" s="43">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="48" t="s">
+        <v>42</v>
+      </c>
       <c r="G20" s="17"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
-      <c r="B21" s="40"/>
+      <c r="B21" s="40">
+        <v>45404</v>
+      </c>
       <c r="C21" s="36"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="48"/>
+      <c r="D21" s="44">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="48" t="s">
+        <v>43</v>
+      </c>
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="39"/>
+      <c r="B22" s="39">
+        <v>45404</v>
+      </c>
       <c r="C22" s="35"/>
-      <c r="D22" s="43"/>
-      <c r="F22" s="48"/>
+      <c r="D22" s="43">
+        <v>30</v>
+      </c>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>44</v>
+      </c>
       <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
-      <c r="B23" s="40"/>
+      <c r="B23" s="40">
+        <v>45404</v>
+      </c>
       <c r="C23" s="36"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="48"/>
+      <c r="D23" s="44">
+        <v>20</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="48" t="s">
+        <v>45</v>
+      </c>
       <c r="G23" s="20"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -8240,7 +8334,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>115</v>
+        <v>295</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8248,7 +8342,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.24652777777777779</v>
+        <v>0.37152777777777779</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8357,7 +8451,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.28819444444444442</v>
+        <v>0.41319444444444442</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8379,6 +8473,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="19" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f3418dd4ca302601ba73fa17965a3f21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns4="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d82fd028d299635ce1df2d808d1b2ae" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8644,18 +8750,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -8665,6 +8759,20 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AC923F-FD8C-4D8C-BC85-CA1561E8B39C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8682,18 +8790,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add the connection to API
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_NardouThomas.xlsx
+++ b/Doc/Journal-de-Travail_NardouThomas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pk88yte\Documents\GitHub\Passion-Book-Mobile\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5092D4-6BAF-4B76-81F4-9780E50CCB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BE33FF-C5CC-4A15-8167-B3099D20EA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -178,6 +178,24 @@
   </si>
   <si>
     <t>Avec M. melly nous avons continuer d'essayer de connecter l'application avec l'API mais sans succès</t>
+  </si>
+  <si>
+    <t>J'ai réussi a connecter mon application avec l'API maintenant il me reste plus qu'a lire mes données</t>
+  </si>
+  <si>
+    <t>J'ai essayé de lire mon json mais sans succès donc je vais essayé d'une autre manière</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai enfin réussi a lire les données de l'API grâce à Tiago qui m'a aidé </t>
+  </si>
+  <si>
+    <t>J'ai modifier mon code pour code pour qu'il accepte le MVVM mais je n'ai pas encore terminé</t>
+  </si>
+  <si>
+    <t>j'ai enfin eu le déclique pour pour pouvoir affichermes livres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai ENFIN réussi à récuperer les informations de l'API et à les afficher sur l'application </t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1090,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.37152777777777779</c:v>
+                  <c:v>0.46180555555555558</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2003,7 +2021,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2074,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 12 heurs 55 minutes</v>
+        <v>0 jours 15 heurs 4 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2075,11 +2093,11 @@
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>355</v>
+        <v>485</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>775</v>
+        <v>905</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2486,52 +2504,91 @@
       </c>
       <c r="G23" s="20"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B24" s="39"/>
       <c r="C24" s="35"/>
-      <c r="D24" s="43"/>
-      <c r="F24" s="48"/>
+      <c r="D24" s="43">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="48" t="s">
+        <v>46</v>
+      </c>
       <c r="G24" s="17"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="40"/>
       <c r="C25" s="36"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="48"/>
+      <c r="D25" s="44">
+        <v>15</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="48" t="s">
+        <v>47</v>
+      </c>
       <c r="G25" s="20"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="39"/>
       <c r="C26" s="35"/>
-      <c r="D26" s="43"/>
-      <c r="F26" s="48"/>
+      <c r="D26" s="43">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="48" t="s">
+        <v>48</v>
+      </c>
       <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="40"/>
       <c r="C27" s="36"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="48"/>
+      <c r="D27" s="44">
+        <v>15</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="48" t="s">
+        <v>49</v>
+      </c>
       <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="39"/>
       <c r="C28" s="35"/>
-      <c r="D28" s="43"/>
-      <c r="F28" s="47"/>
+      <c r="D28" s="43">
+        <v>15</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="47" t="s">
+        <v>50</v>
+      </c>
       <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="40"/>
       <c r="C29" s="36"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="47"/>
+      <c r="D29" s="44">
+        <v>10</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="47" t="s">
+        <v>51</v>
+      </c>
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -8334,7 +8391,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>295</v>
+        <v>425</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8342,7 +8399,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.37152777777777779</v>
+        <v>0.46180555555555558</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8451,7 +8508,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.41319444444444442</v>
+        <v>0.50347222222222221</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8473,18 +8530,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="19" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f3418dd4ca302601ba73fa17965a3f21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns4="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d82fd028d299635ce1df2d808d1b2ae" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8750,6 +8795,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -8759,20 +8816,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AC923F-FD8C-4D8C-BC85-CA1561E8B39C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8790,4 +8833,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add the detection of the book
</commit_message>
<xml_diff>
--- a/Doc/Journal-de-Travail_NardouThomas.xlsx
+++ b/Doc/Journal-de-Travail_NardouThomas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pk88yte\Documents\GitHub\Passion-Book-Mobile\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BE33FF-C5CC-4A15-8167-B3099D20EA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4EFC405-6EF1-4A6B-AD36-4F8617C1C627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t xml:space="preserve">J'ai ENFIN réussi à récuperer les informations de l'API et à les afficher sur l'application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avec M melly nous essayer d'enregistrer le fichier epub </t>
+  </si>
+  <si>
+    <t>j'essaie actuellement de recuperer un livre a partir de son id</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1096,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46180555555555558</c:v>
+                  <c:v>0.52083333333333337</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2021,7 +2027,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2074,7 +2080,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 15 heurs 4 minutes</v>
+        <v>0 jours 16 heurs 30 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2093,11 +2099,11 @@
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>485</v>
+        <v>570</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>905</v>
+        <v>990</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2602,16 +2608,29 @@
       <c r="A31" s="18"/>
       <c r="B31" s="40"/>
       <c r="C31" s="36"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="47"/>
+      <c r="D31" s="44">
+        <v>45</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>52</v>
+      </c>
       <c r="G31" s="20"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B32" s="39"/>
       <c r="C32" s="35"/>
-      <c r="D32" s="43"/>
-      <c r="F32" s="48"/>
+      <c r="D32" s="43">
+        <v>40</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="48" t="s">
+        <v>53</v>
+      </c>
       <c r="G32" s="17"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -8391,7 +8410,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>425</v>
+        <v>510</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8399,7 +8418,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.46180555555555558</v>
+        <v>0.52083333333333337</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8508,7 +8527,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.50347222222222221</v>
+        <v>0.56250000000000011</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8530,6 +8549,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001ABD9BFFC9E543439C53A2705AE306EF" ma:contentTypeVersion="19" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f3418dd4ca302601ba73fa17965a3f21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf2f2df3-a963-4452-b0e7-67dabc627c35" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns4="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5d82fd028d299635ce1df2d808d1b2ae" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
@@ -8795,18 +8826,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="bf2f2df3-a963-4452-b0e7-67dabc627c35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
   <ds:schemaRefs>
@@ -8816,6 +8835,20 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
+    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
+    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
+    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2AC923F-FD8C-4D8C-BC85-CA1561E8B39C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8833,18 +8866,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be0d3259-a7ce-4623-88ec-81594dfcbc1c"/>
-    <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
-    <ds:schemaRef ds:uri="f7d9f5a6-831d-4621-8c77-cbcaf993e406"/>
-    <ds:schemaRef ds:uri="bf2f2df3-a963-4452-b0e7-67dabc627c35"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>